<commit_message>
Created  csv2-b: byrace_w_deceased_continuingPartC in 1_clean  (method)
</commit_message>
<xml_diff>
--- a/Data/use this racial group representation in general population and in EI NATIONAL.xlsx
+++ b/Data/use this racial group representation in general population and in EI NATIONAL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7FE131-02ED-0948-9699-F87247BEAAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E9ADE5-EE42-654D-867D-DE0A39674F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="500" windowWidth="31120" windowHeight="14860" activeTab="1" xr2:uid="{4C1D2749-CBB0-5A44-B45D-6D736832714C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15980" windowHeight="8920" xr2:uid="{4C1D2749-CBB0-5A44-B45D-6D736832714C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1051,10 +1051,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1198,12 +1202,18 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="75000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -2678,16 +2688,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3034,8 +3044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7953D8B6-AFE0-D142-AD30-E1AC282B6005}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3400,7 +3410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF551B1C-9F26-3E4B-AD71-968BD39F901B}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Created 4_plots_or_USRACE_average.qmd and plots for odds ratio for US national dismissal AGAINST the national average, not WHITE
</commit_message>
<xml_diff>
--- a/Data/use this racial group representation in general population and in EI NATIONAL.xlsx
+++ b/Data/use this racial group representation in general population and in EI NATIONAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E9ADE5-EE42-654D-867D-DE0A39674F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E2CAE3-4469-174A-A636-873752E75544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15980" windowHeight="8920" xr2:uid="{4C1D2749-CBB0-5A44-B45D-6D736832714C}"/>
+    <workbookView xWindow="1120" yWindow="7000" windowWidth="25760" windowHeight="15900" xr2:uid="{4C1D2749-CBB0-5A44-B45D-6D736832714C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.10418114000000001</c:v>
+                  <c:v>1.0418113999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.9031740000000002E-2</c:v>
@@ -1157,7 +1157,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.10418114000000001</c:v>
+                  <c:v>1.0418113999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.9031740000000002E-2</c:v>
@@ -1219,6 +1219,64 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.8592103803925666E-3"/>
+                  <c:y val="4.5662100456619328E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="5.2105689253632022E-2"/>
+                      <c:h val="5.0890410958904113E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-DD6A-9B4B-93B6-A68A1F76B4BE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:layout>
@@ -2689,15 +2747,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3044,8 +3102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7953D8B6-AFE0-D142-AD30-E1AC282B6005}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3337,7 +3395,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="3">
-        <v>0.10418114000000001</v>
+        <v>1.0418113999999999E-2</v>
       </c>
       <c r="C15" s="3">
         <v>3.9031740000000002E-2</v>

</xml_diff>

<commit_message>
Excel update - reworked use_this_replacement_racial_group_representation
</commit_message>
<xml_diff>
--- a/Data/use this racial group representation in general population and in EI NATIONAL.xlsx
+++ b/Data/use this racial group representation in general population and in EI NATIONAL.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CAD0F6-97CE-6B40-B485-859F8A6A0704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271EB55D-973D-6B4E-AD04-BC318ED73623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="3400" windowWidth="17700" windowHeight="10100" activeTab="1" xr2:uid="{4C1D2749-CBB0-5A44-B45D-6D736832714C}"/>
+    <workbookView xWindow="8120" yWindow="500" windowWidth="20420" windowHeight="15180" xr2:uid="{4C1D2749-CBB0-5A44-B45D-6D736832714C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" calcOnSave="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Age</t>
   </si>
@@ -50,9 +48,6 @@
   </si>
   <si>
     <t>Hispanic</t>
-  </si>
-  <si>
-    <t>Total + Hispanic Origin</t>
   </si>
   <si>
     <t>White
@@ -123,9 +118,6 @@
     <t>SEE SHEET2 for the data only that  I should import into R!</t>
   </si>
   <si>
-    <t>Black or African American</t>
-  </si>
-  <si>
     <t xml:space="preserve">These numbers are total of 0, 1, 2 year olds divided by the Hispanic &amp; total </t>
   </si>
   <si>
@@ -140,12 +132,26 @@
   <si>
     <t>2020 RATIO for representational chart</t>
   </si>
+  <si>
+    <t>"Non-Hispanic
+White
+alone"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total race + ethnicity (Hispanic White alone/Hispanic origin) </t>
+  </si>
+  <si>
+    <t>sum races</t>
+  </si>
+  <si>
+    <t>sum ethnicity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,6 +218,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Lucida Sans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -417,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -461,6 +473,11 @@
     <xf numFmtId="3" fontId="10" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2768,16 +2785,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2804,16 +2821,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1168400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3160,98 +3177,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7953D8B6-AFE0-D142-AD30-E1AC282B6005}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24">
+      <c r="B1" s="27">
         <v>2020</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="29"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32" t="s">
+        <v>32</v>
+      </c>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="3"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="8">
         <v>3735</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10"/>
+      <c r="D4" s="22">
+        <v>1806.934</v>
+      </c>
+      <c r="E4" s="9">
         <v>970</v>
       </c>
-      <c r="D4" s="10">
-        <v>4705</v>
-      </c>
-      <c r="E4" s="9"/>
       <c r="F4" s="9">
         <v>2597</v>
       </c>
@@ -3270,23 +3294,29 @@
       <c r="K4" s="8">
         <v>246</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="L4" s="11">
+        <f>SUM(F4:K4)</f>
+        <v>3735</v>
+      </c>
+      <c r="M4" s="11">
+        <f>SUM(D4:E4)</f>
+        <v>2776.9340000000002</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="8">
         <v>3774</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10"/>
+      <c r="D5" s="22">
+        <v>1819.2660000000001</v>
+      </c>
+      <c r="E5" s="9">
         <v>986</v>
       </c>
-      <c r="D5" s="10">
-        <v>4760</v>
-      </c>
-      <c r="E5" s="9"/>
       <c r="F5" s="9">
         <v>2623</v>
       </c>
@@ -3305,23 +3335,29 @@
       <c r="K5" s="8">
         <v>244</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="23">
+        <f>SUM(F5:K5)</f>
+        <v>3773</v>
+      </c>
+      <c r="M5" s="11">
+        <f>SUM(D5:E5)</f>
+        <v>2805.2660000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8">
         <v>3853</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="10"/>
+      <c r="D6" s="22">
+        <v>1859.0709999999999</v>
+      </c>
+      <c r="E6" s="9">
         <v>997</v>
       </c>
-      <c r="D6" s="10">
-        <v>4850</v>
-      </c>
-      <c r="E6" s="9"/>
       <c r="F6" s="9">
         <v>2675</v>
       </c>
@@ -3340,21 +3376,34 @@
       <c r="K6" s="8">
         <v>248</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="L6" s="23">
+        <f>SUM(F6:K6)</f>
+        <v>3852</v>
+      </c>
+      <c r="M6" s="11">
+        <f>SUM(D6:E6)</f>
+        <v>2856.0709999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="11">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11">
+        <f>SUM(B4:B6)</f>
+        <v>11362</v>
+      </c>
+      <c r="C7" s="10">
+        <f>SUM(D4:K6)</f>
+        <v>19798.271000000001</v>
+      </c>
+      <c r="D7" s="23">
+        <f>SUM(D4:D6)</f>
+        <v>5485.2709999999997</v>
+      </c>
+      <c r="E7" s="11">
         <v>2953</v>
       </c>
-      <c r="D7" s="10">
-        <v>17268</v>
-      </c>
-      <c r="E7" s="3"/>
       <c r="F7" s="11">
         <v>7895</v>
       </c>
@@ -3373,15 +3422,20 @@
       <c r="K7" s="11">
         <v>738</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="23">
+        <f>SUM(L4:L6)</f>
+        <v>11360</v>
+      </c>
+      <c r="M7" s="11">
+        <f>SUM(M4:M6)</f>
+        <v>8438.2710000000006</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -3396,11 +3450,10 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
         <v>0.17100995999999999</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
       <c r="F9" s="3">
         <v>0.45720408000000001</v>
       </c>
@@ -3423,50 +3476,50 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="22" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="H14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="3">
@@ -3493,7 +3546,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="15">
@@ -3528,36 +3581,36 @@
     </row>
     <row r="19" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="G19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="H19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="I19" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="10">
         <v>17268000</v>
@@ -3586,7 +3639,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="19">
         <v>842413</v>
@@ -3625,202 +3678,4 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF551B1C-9F26-3E4B-AD71-968BD39F901B}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="12">
-        <v>1.26</v>
-      </c>
-      <c r="C2" s="12">
-        <v>3.9</v>
-      </c>
-      <c r="D2" s="12">
-        <v>10.42</v>
-      </c>
-      <c r="E2" s="12">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="F2" s="12">
-        <v>0.24</v>
-      </c>
-      <c r="G2" s="12">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="H2" s="12">
-        <v>45.72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="15">
-        <v>0.69</v>
-      </c>
-      <c r="C3" s="16">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="D3" s="16">
-        <v>12.35</v>
-      </c>
-      <c r="E3" s="16">
-        <v>27.65</v>
-      </c>
-      <c r="F3" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="G3" s="16">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="H3" s="16">
-        <v>50.38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA0A330-6E4D-8642-8692-63C412DD5195}">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1726800</v>
-      </c>
-      <c r="C2">
-        <v>212000</v>
-      </c>
-      <c r="D2">
-        <v>674000</v>
-      </c>
-      <c r="E2">
-        <v>1799000</v>
-      </c>
-      <c r="F2">
-        <v>2953000</v>
-      </c>
-      <c r="G2">
-        <v>42000</v>
-      </c>
-      <c r="H2">
-        <v>738000</v>
-      </c>
-      <c r="I2">
-        <v>7895000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="19">
-        <v>842413</v>
-      </c>
-      <c r="C3" s="19">
-        <v>5842</v>
-      </c>
-      <c r="D3" s="19">
-        <v>36966</v>
-      </c>
-      <c r="E3" s="19">
-        <v>104046</v>
-      </c>
-      <c r="F3" s="19">
-        <v>232969</v>
-      </c>
-      <c r="G3" s="19">
-        <v>2557</v>
-      </c>
-      <c r="H3" s="19">
-        <v>35650</v>
-      </c>
-      <c r="I3" s="20">
-        <v>424383</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>